<commit_message>
M3 Cord Production System #955 - Implements Export S8 #3
</commit_message>
<xml_diff>
--- a/05.Controls/M3.Cord.Controls/Resources/Excels/DIP_Confirmaion_condition.xlsx
+++ b/05.Controls/M3.Cord.Controls/Resources/Excels/DIP_Confirmaion_condition.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>CONFIRMATION CONDITION CHECK SHEET</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Item :</t>
   </si>
   <si>
-    <t>P1671TT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date </t>
   </si>
   <si>
@@ -116,84 +113,30 @@
     <t>1.1 Cord structure (โครงสร้างเชือก)</t>
   </si>
   <si>
-    <t>[SC]</t>
-  </si>
-  <si>
-    <t>P 1670T / 1</t>
-  </si>
-  <si>
     <t>1.2 Yarn type (ชนิดด้าย)</t>
   </si>
   <si>
-    <t>1670T- 360- 705 M</t>
-  </si>
-  <si>
-    <t>1670T - 360 - 705 M</t>
-  </si>
-  <si>
     <t>1.3 1st twist (การตีเกลียวครั้งที่ 1)</t>
   </si>
   <si>
-    <t>80.0 + 10.0 ( S ) T/M</t>
-  </si>
-  <si>
     <t>1.4 2nd twist (การตีเกลียวครั้งที่ 2)</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>1.5 Shape of yarn(รูปร่างของด้าย)</t>
-  </si>
-  <si>
-    <t>Paper Tube</t>
-  </si>
-  <si>
     <t>1.6 Weight (Kg) น้ำหนัก (กก.)</t>
   </si>
   <si>
-    <r>
-      <t>5.0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.2</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">2. creel setting </t>
   </si>
   <si>
     <t>2.1 Use tensor (ให้น้ำหนักทับ)</t>
   </si>
   <si>
-    <t>ใช้</t>
-  </si>
-  <si>
     <t>2.2 Knot Condition (สภาวะการต่อด้าย)</t>
   </si>
   <si>
-    <t xml:space="preserve">Air splicer </t>
-  </si>
-  <si>
     <t>2.3 ตัวดักปม ( Slub catswe )</t>
   </si>
   <si>
-    <t>0.50 MM</t>
-  </si>
-  <si>
     <t xml:space="preserve">CS-8 Cordseter </t>
   </si>
   <si>
@@ -203,57 +146,12 @@
     <t>3.1 Stretch  Dryer (%การยืด ช่วงทำให้แห้ง)</t>
   </si>
   <si>
-    <t>101.0± 0.2</t>
-  </si>
-  <si>
     <t>3.2 Stretch Hot ( %การยืด ช่วงร้อน)</t>
   </si>
   <si>
-    <r>
-      <t>102.5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 0.2</t>
-    </r>
-  </si>
-  <si>
     <t>3.3 Stretch Normal( %การยืด ช่วงปกติ)</t>
   </si>
   <si>
-    <r>
-      <t>99.0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 0.2 </t>
-    </r>
-  </si>
-  <si>
     <t>3.4 Stretch Total ( %การยืด รวม)</t>
   </si>
   <si>
@@ -263,51 +161,9 @@
     <t>Temp  Dryer  (อุณหภูมิ ช่วงทำให้แห้ง)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">150 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
     <t>Temp  Hot (อุณหภูมิ ช่วงร้อน)</t>
   </si>
   <si>
-    <r>
-      <t>242</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 3 </t>
-    </r>
-  </si>
-  <si>
     <t>Temp  Normal ( อุณหภูมิช่วงปกติ)</t>
   </si>
   <si>
@@ -321,9 +177,6 @@
   </si>
   <si>
     <t>6.1 Speed (m/min)(ความเร็วรอบ)</t>
-  </si>
-  <si>
-    <t>40±0.5</t>
   </si>
   <si>
     <t xml:space="preserve">7. No. of cord </t>
@@ -339,9 +192,6 @@
     <t>8.1 Sofnor(ปรับให้นิ่ม)</t>
   </si>
   <si>
-    <t>ON  (เปิด)</t>
-  </si>
-  <si>
     <t>8.2 Draw nip(ลูกกลิ้งกด)</t>
   </si>
   <si>
@@ -349,9 +199,6 @@
   </si>
   <si>
     <t>9.1 Solution name(Concentration) (ความเข้มข้น)</t>
-  </si>
-  <si>
-    <t>CT   7 - 1   (27.5 %)</t>
   </si>
   <si>
     <t xml:space="preserve">  อ่าง 1.</t>
@@ -401,56 +248,8 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">2.3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 0.3</t>
-    </r>
-  </si>
-  <si>
-    <t>2.3 + 0.3</t>
-  </si>
-  <si>
     <t>9.4 WPU standard (%) 
 (มาตรฐานการดูดซับน้ำยา)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">26 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 2 % </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">26 + 2 % </t>
   </si>
   <si>
     <t xml:space="preserve">10. Dipping No 2 </t>
@@ -506,9 +305,6 @@
     </r>
   </si>
   <si>
-    <t>Free</t>
-  </si>
-  <si>
     <t>10.4 WPU standard (%) 
 (มาตรฐานการดูดซับน้ำยา)</t>
   </si>
@@ -525,61 +321,25 @@
     <t>11.2 Contrn presure ปรับลม</t>
   </si>
   <si>
-    <t>0.26 Mpa</t>
-  </si>
-  <si>
     <t xml:space="preserve">11.3 Spring tension ปรับสปริง  </t>
   </si>
   <si>
-    <t xml:space="preserve"> 30 MM</t>
-  </si>
-  <si>
     <t>11.4 Peper Tube color (หลอดสี)</t>
   </si>
   <si>
-    <t>สีส้ม</t>
-  </si>
-  <si>
     <t>11.5 Cheese weight (kg) น้ำหนักลูกด้าย</t>
   </si>
   <si>
-    <r>
-      <t>5.1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.2</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">12.Circulation </t>
   </si>
   <si>
     <t>12.1 Circulation Zone 1,2</t>
   </si>
   <si>
-    <t xml:space="preserve"> 45  Hz.   </t>
-  </si>
-  <si>
     <t xml:space="preserve">13. Exhaust  </t>
   </si>
   <si>
     <t>13.1  Exhaust Zone 1,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20  Hz.   </t>
   </si>
   <si>
     <t>14.Exhaust  Fan</t>
@@ -589,18 +349,12 @@
  ( พัดลมดูดควัน หน้า หลัง)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 40  Hz.   </t>
-  </si>
-  <si>
     <t>15.Spong</t>
   </si>
   <si>
     <t xml:space="preserve"> 15.1 Spong (ฟองน้ำ)</t>
   </si>
   <si>
-    <t>Use</t>
-  </si>
-  <si>
     <t>FM-CS…...  Effective date  : …………..        Approved by : CS</t>
   </si>
   <si>
@@ -614,6 +368,9 @@
   </si>
   <si>
     <t>Leader shift / หัวหน้ากะ</t>
+  </si>
+  <si>
+    <t>1.5 Label of yarn(ลาเบลชี้บ่งบนลูกด้าย)</t>
   </si>
 </sst>
 </file>
@@ -624,7 +381,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,16 +435,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="18"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
@@ -1749,7 +1496,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1920,32 +1667,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1975,19 +1722,67 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="68" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="69" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2074,62 +1869,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="68" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2171,7 +1918,7 @@
         <xdr:cNvPr id="2" name="Picture 25" descr="logo.JPG">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9EAA84F-43C3-444A-B43B-F2367591E060}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9EAA84F-43C3-444A-B43B-F2367591E060}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2223,7 +1970,7 @@
         <xdr:cNvPr id="3" name="Picture 27" descr="logo.JPG">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{480374C2-6B59-4D60-A7DC-50C1397F604D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480374C2-6B59-4D60-A7DC-50C1397F604D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2548,7 +2295,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2562,7 +2309,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="29.25" customHeight="1"/>
@@ -2580,50 +2327,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="44.25" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="178" t="s">
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="180"/>
+      <c r="J1" s="149"/>
     </row>
     <row r="2" spans="1:10" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A2" s="181" t="s">
+      <c r="A2" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="184" t="s">
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="185"/>
+      <c r="J2" s="154"/>
     </row>
     <row r="3" spans="1:10" ht="24.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -2632,34 +2377,34 @@
     <row r="4" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="20.25" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="155" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="157"/>
+      <c r="G5" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="186" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="187"/>
-      <c r="D5" s="187"/>
-      <c r="E5" s="187"/>
-      <c r="F5" s="188"/>
-      <c r="G5" s="14" t="s">
-        <v>11</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -2667,588 +2412,464 @@
     </row>
     <row r="6" spans="1:10" ht="20.25" customHeight="1" thickBot="1">
       <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="158"/>
+      <c r="C6" s="159"/>
+      <c r="D6" s="159"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="189"/>
-      <c r="C6" s="190"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="190"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="17" t="s">
-        <v>13</v>
-      </c>
       <c r="H6" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="33.75" customHeight="1">
-      <c r="A7" s="163" t="s">
+      <c r="A7" s="179" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="180"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="180"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="167" t="s">
+      <c r="G7" s="185" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="169" t="s">
+      <c r="H7" s="181"/>
+      <c r="I7" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="165"/>
-      <c r="I7" s="169" t="s">
+      <c r="J7" s="186"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1">
+      <c r="A8" s="166"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="167"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="187" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="170"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1">
-      <c r="A8" s="150"/>
-      <c r="B8" s="151"/>
-      <c r="C8" s="151"/>
-      <c r="D8" s="151"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="168"/>
-      <c r="G8" s="171" t="s">
+      <c r="H8" s="188"/>
+      <c r="I8" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="172"/>
-      <c r="I8" s="148" t="s">
+      <c r="J8" s="165"/>
+    </row>
+    <row r="9" spans="1:10" ht="36" customHeight="1" thickBot="1">
+      <c r="A9" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="149"/>
-    </row>
-    <row r="9" spans="1:10" ht="36" customHeight="1" thickBot="1">
-      <c r="A9" s="150" t="s">
+      <c r="B9" s="167"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="151"/>
-      <c r="C9" s="151"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="151"/>
-      <c r="F9" s="168"/>
-      <c r="G9" s="20" t="s">
+      <c r="H9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="I9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="J9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="22" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="31.5" customHeight="1" thickTop="1">
+      <c r="A10" s="168" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A10" s="152" t="s">
+      <c r="B10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="C10" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
-      <c r="F10" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>29</v>
-      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="28"/>
-      <c r="I10" s="27" t="s">
-        <v>29</v>
-      </c>
+      <c r="I10" s="27"/>
       <c r="J10" s="29"/>
     </row>
     <row r="11" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A11" s="153"/>
+      <c r="A11" s="169"/>
       <c r="B11" s="30"/>
       <c r="C11" s="31" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>31</v>
-      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="34" t="s">
-        <v>32</v>
-      </c>
+      <c r="I11" s="34"/>
       <c r="J11" s="36"/>
     </row>
     <row r="12" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A12" s="153"/>
+      <c r="A12" s="169"/>
       <c r="B12" s="30"/>
       <c r="C12" s="31" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>34</v>
-      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="35"/>
-      <c r="I12" s="34" t="s">
-        <v>34</v>
-      </c>
+      <c r="I12" s="34"/>
       <c r="J12" s="36"/>
     </row>
     <row r="13" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A13" s="153"/>
+      <c r="A13" s="169"/>
       <c r="B13" s="30"/>
       <c r="C13" s="31" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="37" t="s">
-        <v>36</v>
-      </c>
+      <c r="G13" s="37"/>
       <c r="H13" s="35"/>
-      <c r="I13" s="37" t="s">
-        <v>36</v>
-      </c>
+      <c r="I13" s="37"/>
       <c r="J13" s="36"/>
     </row>
     <row r="14" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A14" s="153"/>
+      <c r="A14" s="169"/>
       <c r="B14" s="30"/>
       <c r="C14" s="31" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
-      <c r="G14" s="143" t="s">
-        <v>38</v>
-      </c>
+      <c r="G14" s="143"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="143" t="s">
-        <v>38</v>
-      </c>
+      <c r="I14" s="143"/>
       <c r="J14" s="36"/>
     </row>
     <row r="15" spans="1:10" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A15" s="153"/>
+      <c r="A15" s="169"/>
       <c r="B15" s="38"/>
       <c r="C15" s="39" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
       <c r="F15" s="41"/>
-      <c r="G15" s="42" t="s">
-        <v>40</v>
-      </c>
+      <c r="G15" s="42"/>
       <c r="H15" s="43"/>
-      <c r="I15" s="42" t="s">
-        <v>40</v>
-      </c>
+      <c r="I15" s="42"/>
       <c r="J15" s="44"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A16" s="153"/>
+      <c r="A16" s="169"/>
       <c r="B16" s="30" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="46"/>
       <c r="F16" s="47"/>
-      <c r="G16" s="48" t="s">
-        <v>43</v>
-      </c>
+      <c r="G16" s="48"/>
       <c r="H16" s="49"/>
-      <c r="I16" s="48" t="s">
-        <v>43</v>
-      </c>
+      <c r="I16" s="48"/>
       <c r="J16" s="50"/>
     </row>
     <row r="17" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A17" s="153"/>
+      <c r="A17" s="169"/>
       <c r="B17" s="30"/>
       <c r="C17" s="31" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="32"/>
       <c r="F17" s="33"/>
-      <c r="G17" s="143" t="s">
-        <v>45</v>
-      </c>
+      <c r="G17" s="143"/>
       <c r="H17" s="35"/>
-      <c r="I17" s="143" t="s">
-        <v>45</v>
-      </c>
+      <c r="I17" s="143"/>
       <c r="J17" s="36"/>
     </row>
     <row r="18" spans="1:14" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A18" s="154"/>
+      <c r="A18" s="170"/>
       <c r="B18" s="38"/>
       <c r="C18" s="39" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D18" s="52"/>
       <c r="E18" s="40"/>
       <c r="F18" s="41"/>
-      <c r="G18" s="53" t="s">
-        <v>47</v>
-      </c>
+      <c r="G18" s="53"/>
       <c r="H18" s="43"/>
-      <c r="I18" s="53" t="s">
-        <v>47</v>
-      </c>
+      <c r="I18" s="53"/>
       <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:14" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A19" s="155" t="s">
-        <v>48</v>
+      <c r="A19" s="171" t="s">
+        <v>35</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
-      <c r="F19" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="55" t="s">
-        <v>51</v>
-      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="55"/>
       <c r="H19" s="48"/>
-      <c r="I19" s="55" t="s">
-        <v>51</v>
-      </c>
+      <c r="I19" s="55"/>
       <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A20" s="155"/>
+      <c r="A20" s="171"/>
       <c r="B20" s="30"/>
       <c r="C20" s="56" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="57" t="s">
-        <v>53</v>
-      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="34"/>
-      <c r="I20" s="57" t="s">
-        <v>53</v>
-      </c>
+      <c r="I20" s="57"/>
       <c r="J20" s="36"/>
       <c r="L20" s="58"/>
       <c r="M20" s="59"/>
       <c r="N20" s="60"/>
     </row>
     <row r="21" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A21" s="155"/>
+      <c r="A21" s="171"/>
       <c r="B21" s="30"/>
       <c r="C21" s="56" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="57" t="s">
-        <v>55</v>
-      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="34"/>
-      <c r="I21" s="57" t="s">
-        <v>55</v>
-      </c>
+      <c r="I21" s="57"/>
       <c r="J21" s="36"/>
     </row>
     <row r="22" spans="1:14" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A22" s="155"/>
+      <c r="A22" s="171"/>
       <c r="B22" s="38"/>
       <c r="C22" s="61" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="62">
-        <v>102.5</v>
-      </c>
+      <c r="G22" s="62"/>
       <c r="H22" s="53"/>
-      <c r="I22" s="62">
-        <v>102.5</v>
-      </c>
+      <c r="I22" s="62"/>
       <c r="J22" s="44"/>
     </row>
     <row r="23" spans="1:14" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A23" s="155"/>
+      <c r="A23" s="171"/>
       <c r="B23" s="30" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D23" s="46"/>
       <c r="E23" s="63"/>
-      <c r="F23" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="65" t="s">
-        <v>59</v>
-      </c>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="66"/>
-      <c r="I23" s="65" t="s">
-        <v>59</v>
-      </c>
+      <c r="I23" s="65"/>
       <c r="J23" s="67"/>
     </row>
     <row r="24" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A24" s="155"/>
+      <c r="A24" s="171"/>
       <c r="B24" s="30"/>
       <c r="C24" s="56" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="68"/>
-      <c r="F24" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="70" t="s">
-        <v>61</v>
-      </c>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
       <c r="H24" s="71"/>
-      <c r="I24" s="70" t="s">
-        <v>61</v>
-      </c>
+      <c r="I24" s="70"/>
       <c r="J24" s="72"/>
     </row>
     <row r="25" spans="1:14" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A25" s="155"/>
+      <c r="A25" s="171"/>
       <c r="B25" s="38"/>
       <c r="C25" s="61" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D25" s="40"/>
       <c r="E25" s="73"/>
-      <c r="F25" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="75" t="s">
-        <v>61</v>
-      </c>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
       <c r="H25" s="76"/>
-      <c r="I25" s="75" t="s">
-        <v>61</v>
-      </c>
+      <c r="I25" s="75"/>
       <c r="J25" s="77"/>
     </row>
     <row r="26" spans="1:14" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A26" s="155"/>
+      <c r="A26" s="171"/>
       <c r="B26" s="30" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C26" s="78" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D26" s="46"/>
       <c r="E26" s="63"/>
       <c r="F26" s="64"/>
-      <c r="G26" s="65">
-        <v>29000</v>
-      </c>
+      <c r="G26" s="65"/>
       <c r="H26" s="66"/>
-      <c r="I26" s="65">
-        <v>29000</v>
-      </c>
+      <c r="I26" s="65"/>
       <c r="J26" s="67"/>
     </row>
     <row r="27" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A27" s="155"/>
+      <c r="A27" s="171"/>
       <c r="B27" s="79" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D27" s="80"/>
       <c r="E27" s="81"/>
       <c r="F27" s="69"/>
-      <c r="G27" s="35" t="s">
-        <v>67</v>
-      </c>
+      <c r="G27" s="35"/>
       <c r="H27" s="71"/>
-      <c r="I27" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J27" s="72" t="s">
-        <v>36</v>
-      </c>
+      <c r="I27" s="35"/>
+      <c r="J27" s="72"/>
     </row>
     <row r="28" spans="1:14" ht="41.25" customHeight="1">
-      <c r="A28" s="155"/>
+      <c r="A28" s="171"/>
       <c r="B28" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="157" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="158"/>
-      <c r="E28" s="159"/>
+        <v>49</v>
+      </c>
+      <c r="C28" s="173" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="174"/>
+      <c r="E28" s="175"/>
       <c r="F28" s="69"/>
-      <c r="G28" s="35">
-        <v>148</v>
-      </c>
+      <c r="G28" s="35"/>
       <c r="H28" s="71"/>
-      <c r="I28" s="35">
-        <v>148</v>
-      </c>
-      <c r="J28" s="72" t="s">
-        <v>36</v>
-      </c>
+      <c r="I28" s="35"/>
+      <c r="J28" s="72"/>
     </row>
     <row r="29" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A29" s="155"/>
+      <c r="A29" s="171"/>
       <c r="B29" s="30" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D29" s="80"/>
       <c r="E29" s="81"/>
       <c r="F29" s="69"/>
-      <c r="G29" s="35" t="s">
-        <v>72</v>
-      </c>
+      <c r="G29" s="35"/>
       <c r="H29" s="71"/>
-      <c r="I29" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="J29" s="72" t="s">
-        <v>36</v>
-      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="72"/>
     </row>
     <row r="30" spans="1:14" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A30" s="155"/>
+      <c r="A30" s="171"/>
       <c r="B30" s="82"/>
       <c r="C30" s="39" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D30" s="83"/>
       <c r="E30" s="84"/>
       <c r="F30" s="74"/>
-      <c r="G30" s="43" t="s">
-        <v>72</v>
-      </c>
+      <c r="G30" s="43"/>
       <c r="H30" s="76"/>
-      <c r="I30" s="43" t="s">
-        <v>72</v>
-      </c>
+      <c r="I30" s="43"/>
       <c r="J30" s="77"/>
     </row>
     <row r="31" spans="1:14" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A31" s="155"/>
+      <c r="A31" s="171"/>
       <c r="B31" s="79" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D31" s="85"/>
       <c r="E31" s="86"/>
       <c r="F31" s="64"/>
-      <c r="G31" s="49" t="s">
-        <v>76</v>
-      </c>
+      <c r="G31" s="49"/>
       <c r="H31" s="66"/>
-      <c r="I31" s="49" t="s">
-        <v>76</v>
-      </c>
+      <c r="I31" s="49"/>
       <c r="J31" s="67"/>
     </row>
     <row r="32" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A32" s="155"/>
+      <c r="A32" s="171"/>
       <c r="B32" s="87" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D32" s="88"/>
       <c r="E32" s="89"/>
       <c r="F32" s="69"/>
-      <c r="G32" s="34">
-        <v>1</v>
-      </c>
+      <c r="G32" s="34"/>
       <c r="H32" s="71"/>
-      <c r="I32" s="34">
-        <v>1</v>
-      </c>
+      <c r="I32" s="34"/>
       <c r="J32" s="72"/>
     </row>
     <row r="33" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A33" s="155"/>
+      <c r="A33" s="171"/>
       <c r="B33" s="87"/>
       <c r="C33" s="90" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D33" s="91"/>
       <c r="E33" s="92"/>
       <c r="F33" s="93"/>
-      <c r="G33" s="94" t="s">
-        <v>80</v>
-      </c>
+      <c r="G33" s="94"/>
       <c r="H33" s="95"/>
-      <c r="I33" s="94" t="s">
-        <v>81</v>
-      </c>
+      <c r="I33" s="94"/>
       <c r="J33" s="96"/>
     </row>
     <row r="34" spans="1:10" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A34" s="155"/>
+      <c r="A34" s="171"/>
       <c r="B34" s="82"/>
-      <c r="C34" s="160" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="161"/>
-      <c r="E34" s="162"/>
+      <c r="C34" s="176" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="177"/>
+      <c r="E34" s="178"/>
       <c r="F34" s="74"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
-      </c>
+      <c r="G34" s="43"/>
       <c r="H34" s="76"/>
-      <c r="I34" s="43" t="s">
-        <v>84</v>
-      </c>
+      <c r="I34" s="43"/>
       <c r="J34" s="77"/>
     </row>
     <row r="35" spans="1:10" ht="31.5" customHeight="1" thickTop="1">
-      <c r="A35" s="155"/>
+      <c r="A35" s="171"/>
       <c r="B35" s="79" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D35" s="85"/>
       <c r="E35" s="86"/>
@@ -3259,51 +2880,43 @@
       <c r="J35" s="67"/>
     </row>
     <row r="36" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A36" s="155"/>
+      <c r="A36" s="171"/>
       <c r="B36" s="87" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D36" s="88"/>
       <c r="E36" s="89"/>
       <c r="F36" s="69"/>
-      <c r="G36" s="35">
-        <v>0</v>
-      </c>
+      <c r="G36" s="35"/>
       <c r="H36" s="71"/>
-      <c r="I36" s="35">
-        <v>0</v>
-      </c>
+      <c r="I36" s="35"/>
       <c r="J36" s="72"/>
     </row>
     <row r="37" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A37" s="155"/>
+      <c r="A37" s="171"/>
       <c r="B37" s="87"/>
       <c r="C37" s="90" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="D37" s="91"/>
       <c r="E37" s="92"/>
       <c r="F37" s="93"/>
-      <c r="G37" s="94" t="s">
-        <v>90</v>
-      </c>
+      <c r="G37" s="94"/>
       <c r="H37" s="95"/>
-      <c r="I37" s="94" t="s">
-        <v>90</v>
-      </c>
+      <c r="I37" s="94"/>
       <c r="J37" s="96"/>
     </row>
     <row r="38" spans="1:10" ht="48" customHeight="1" thickBot="1">
-      <c r="A38" s="156"/>
+      <c r="A38" s="172"/>
       <c r="B38" s="82"/>
-      <c r="C38" s="160" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="161"/>
-      <c r="E38" s="162"/>
+      <c r="C38" s="176" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="177"/>
+      <c r="E38" s="178"/>
       <c r="F38" s="74"/>
       <c r="G38" s="43"/>
       <c r="H38" s="76"/>
@@ -3312,176 +2925,140 @@
     </row>
     <row r="39" spans="1:10" ht="31.5" customHeight="1" thickTop="1">
       <c r="A39" s="97" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B39" s="87" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C39" s="98" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="D39" s="99"/>
       <c r="E39" s="100"/>
       <c r="F39" s="64"/>
-      <c r="G39" s="101">
-        <v>2.9952000000000001</v>
-      </c>
+      <c r="G39" s="101"/>
       <c r="H39" s="66"/>
-      <c r="I39" s="101">
-        <v>2.9952000000000001</v>
-      </c>
+      <c r="I39" s="101"/>
       <c r="J39" s="67"/>
     </row>
     <row r="40" spans="1:10" ht="31.5" customHeight="1">
       <c r="A40" s="102"/>
       <c r="B40" s="87"/>
       <c r="C40" s="103" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D40" s="104"/>
       <c r="E40" s="105"/>
       <c r="F40" s="106"/>
-      <c r="G40" s="35" t="s">
-        <v>96</v>
-      </c>
+      <c r="G40" s="35"/>
       <c r="H40" s="71"/>
-      <c r="I40" s="35" t="s">
-        <v>96</v>
-      </c>
+      <c r="I40" s="35"/>
       <c r="J40" s="72"/>
     </row>
     <row r="41" spans="1:10" ht="31.5" customHeight="1">
       <c r="A41" s="102"/>
       <c r="B41" s="87"/>
       <c r="C41" s="103" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="D41" s="104"/>
       <c r="E41" s="105"/>
       <c r="F41" s="107"/>
-      <c r="G41" s="68" t="s">
-        <v>98</v>
-      </c>
+      <c r="G41" s="68"/>
       <c r="H41" s="71"/>
-      <c r="I41" s="68" t="s">
-        <v>98</v>
-      </c>
+      <c r="I41" s="68"/>
       <c r="J41" s="108"/>
     </row>
     <row r="42" spans="1:10" ht="31.5" customHeight="1">
       <c r="A42" s="102"/>
       <c r="B42" s="87"/>
       <c r="C42" s="109" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="D42" s="110"/>
       <c r="E42" s="111"/>
       <c r="F42" s="112"/>
-      <c r="G42" s="144" t="s">
-        <v>100</v>
-      </c>
+      <c r="G42" s="144"/>
       <c r="H42" s="95"/>
-      <c r="I42" s="144" t="s">
-        <v>100</v>
-      </c>
+      <c r="I42" s="144"/>
       <c r="J42" s="113"/>
     </row>
     <row r="43" spans="1:10" ht="38.25" customHeight="1" thickBot="1">
       <c r="A43" s="114"/>
       <c r="B43" s="82"/>
       <c r="C43" s="115" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="D43" s="83"/>
       <c r="E43" s="84"/>
       <c r="F43" s="74"/>
-      <c r="G43" s="42" t="s">
-        <v>102</v>
-      </c>
+      <c r="G43" s="42"/>
       <c r="H43" s="76"/>
-      <c r="I43" s="42" t="s">
-        <v>102</v>
-      </c>
+      <c r="I43" s="42"/>
       <c r="J43" s="116"/>
     </row>
     <row r="44" spans="1:10" ht="31.5" customHeight="1" thickTop="1">
       <c r="A44" s="102"/>
       <c r="B44" s="30" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D44" s="118"/>
       <c r="E44" s="119"/>
       <c r="F44" s="120"/>
-      <c r="G44" s="49" t="s">
-        <v>105</v>
-      </c>
+      <c r="G44" s="49"/>
       <c r="H44" s="66"/>
-      <c r="I44" s="49" t="s">
-        <v>105</v>
-      </c>
+      <c r="I44" s="49"/>
       <c r="J44" s="121"/>
     </row>
     <row r="45" spans="1:10" ht="31.5" customHeight="1">
       <c r="A45" s="102"/>
       <c r="B45" s="30" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C45" s="122" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="D45" s="123"/>
       <c r="E45" s="124"/>
       <c r="F45" s="125"/>
-      <c r="G45" s="35" t="s">
-        <v>108</v>
-      </c>
+      <c r="G45" s="35"/>
       <c r="H45" s="71"/>
-      <c r="I45" s="35" t="s">
-        <v>108</v>
-      </c>
+      <c r="I45" s="35"/>
       <c r="J45" s="108"/>
     </row>
     <row r="46" spans="1:10" ht="78" customHeight="1">
       <c r="A46" s="102"/>
       <c r="B46" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="173" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="174"/>
-      <c r="E46" s="175"/>
+        <v>77</v>
+      </c>
+      <c r="C46" s="189" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="190"/>
+      <c r="E46" s="191"/>
       <c r="F46" s="107"/>
-      <c r="G46" s="35" t="s">
-        <v>111</v>
-      </c>
+      <c r="G46" s="35"/>
       <c r="H46" s="80"/>
-      <c r="I46" s="35" t="s">
-        <v>111</v>
-      </c>
+      <c r="I46" s="35"/>
       <c r="J46" s="108"/>
     </row>
     <row r="47" spans="1:10" ht="31.5" customHeight="1">
       <c r="A47" s="102"/>
       <c r="B47" s="30" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C47" s="126" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="D47" s="127"/>
       <c r="E47" s="128"/>
       <c r="F47" s="69"/>
-      <c r="G47" s="35" t="s">
-        <v>114</v>
-      </c>
+      <c r="G47" s="35"/>
       <c r="H47" s="80"/>
-      <c r="I47" s="35" t="s">
-        <v>114</v>
-      </c>
+      <c r="I47" s="35"/>
       <c r="J47" s="108"/>
     </row>
     <row r="48" spans="1:10" ht="31.5" customHeight="1" thickBot="1">
@@ -3498,30 +3075,30 @@
     </row>
     <row r="49" spans="1:10" ht="24.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="E49" s="138"/>
       <c r="F49" s="139"/>
-      <c r="G49" s="176" t="s">
-        <v>116</v>
-      </c>
-      <c r="H49" s="177"/>
-      <c r="I49" s="176" t="s">
-        <v>117</v>
-      </c>
-      <c r="J49" s="177"/>
+      <c r="G49" s="145" t="s">
+        <v>82</v>
+      </c>
+      <c r="H49" s="146"/>
+      <c r="I49" s="145" t="s">
+        <v>83</v>
+      </c>
+      <c r="J49" s="146"/>
     </row>
     <row r="50" spans="1:10" ht="24.75" customHeight="1">
       <c r="E50" s="138"/>
       <c r="F50" s="139"/>
-      <c r="G50" s="145" t="s">
-        <v>118</v>
-      </c>
-      <c r="H50" s="146"/>
-      <c r="I50" s="145" t="s">
-        <v>119</v>
-      </c>
-      <c r="J50" s="146"/>
+      <c r="G50" s="161" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="162"/>
+      <c r="I50" s="161" t="s">
+        <v>85</v>
+      </c>
+      <c r="J50" s="162"/>
     </row>
     <row r="51" spans="1:10" ht="79.5" customHeight="1" thickBot="1">
       <c r="E51" s="138"/>
@@ -3536,18 +3113,11 @@
       <c r="F52" s="139"/>
       <c r="G52" s="138"/>
       <c r="H52" s="138"/>
-      <c r="I52" s="147"/>
-      <c r="J52" s="147"/>
+      <c r="I52" s="163"/>
+      <c r="J52" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B5:F6"/>
     <mergeCell ref="G50:H50"/>
     <mergeCell ref="I50:J50"/>
     <mergeCell ref="I52:J52"/>
@@ -3564,6 +3134,13 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="C46:E46"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B5:F6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>